<commit_message>
Made changes in reading excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D825961E-25B8-45C6-90AB-2882F4218FCF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED3FE9-A35C-49CD-B490-43FFA1788FD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="2955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="2955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One-way" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -480,12 +480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64D6F29-2C0A-4B04-8FA8-EE32F626725A}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added code for API validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED3FE9-A35C-49CD-B490-43FFA1788FD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{530AD920-FDDF-4108-B6F7-975B8F6320EA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13770" windowHeight="2955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="2925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="One-way" sheetId="1" r:id="rId1"/>
     <sheet name="Round-trip" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,9 +45,6 @@
     <t>Mumbai</t>
   </si>
   <si>
-    <t>22/10/2018</t>
-  </si>
-  <si>
     <t>Adults</t>
   </si>
   <si>
@@ -59,7 +57,10 @@
     <t>Return On</t>
   </si>
   <si>
-    <t>30/10/2018</t>
+    <t>22/12/2018</t>
+  </si>
+  <si>
+    <t>30/12/2018</t>
   </si>
 </sst>
 </file>
@@ -405,7 +406,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,12 +444,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -456,7 +457,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -464,7 +465,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -481,7 +482,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,12 +520,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -532,7 +533,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
@@ -540,7 +541,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -548,7 +549,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>

</xml_diff>